<commit_message>
Artefato 18 e ortografia do 17
</commit_message>
<xml_diff>
--- a/17. Análise de eventos.xlsx
+++ b/17. Análise de eventos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela\Documents\3  Semestre\OPE\RoadOn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giovanna Rocha\Desktop\Pessoal\Faculdade\Terceiro Semestre\ENGENHARIA DE REQUISITOS\RoadOn\RoadOn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE2CB7B-0EEF-415C-A801-0F1B007E7765}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6CCA8B-FF1D-4EEB-A1D5-E2B0646F9534}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -172,9 +172,6 @@
     <t>Agente de vendas disponibiliza excursão.</t>
   </si>
   <si>
-    <t>Cliente solicira o cancelamento da excursão.</t>
-  </si>
-  <si>
     <t>Cliente envia recibo de pagamento</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>Gerente solicita sugestão</t>
+  </si>
+  <si>
+    <t>Cliente solicita o cancelamento da excursão.</t>
   </si>
 </sst>
 </file>
@@ -314,33 +314,6 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -394,6 +367,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,367 +799,367 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="3" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="9" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9" t="s">
+      <c r="H3" s="25"/>
+      <c r="I3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
     </row>
     <row r="5" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="14" t="s">
+      <c r="D5" s="26"/>
+      <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
     </row>
     <row r="6" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="6">
         <v>1</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="7"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="15">
+      <c r="C7" s="27"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="6">
         <v>2</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="10"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="1"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="15">
+      <c r="C8" s="27"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="6">
         <v>3</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="10"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="1"/>
     </row>
     <row r="9" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="15">
+      <c r="C9" s="27"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="6">
         <v>4</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="10"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="1"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="7"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="15">
+      <c r="C10" s="27"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="6">
         <v>5</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="10"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="1"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="7"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="15">
+      <c r="C11" s="27"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="6">
         <v>6</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17" t="s">
+      <c r="G11" s="8"/>
+      <c r="H11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="10"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="1"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="7"/>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="6">
         <v>7</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="18" t="s">
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C13" s="7"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="15">
+      <c r="C13" s="27"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="6">
         <v>8</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="18" t="s">
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
     </row>
     <row r="14" spans="3:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="6">
         <v>1</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="18" t="s">
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="10"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="1"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="15">
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="6">
         <v>2</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="18" t="s">
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="10"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="1"/>
     </row>
     <row r="16" spans="3:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="14">
         <v>1</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17" t="s">
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="4"/>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="24"/>
+      <c r="D17" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="16">
         <v>2</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="10"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="1"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="23">
+      <c r="C18" s="24"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="14">
         <v>3</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17" t="s">
+      <c r="G18" s="8"/>
+      <c r="H18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="10"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:K4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="D12:D13"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="G3:H4"/>
-    <mergeCell ref="I3:K4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1170,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,324 +1190,324 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="10"/>
-      <c r="F2" s="9" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="F2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="10"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="10"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="14" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="10"/>
+      <c r="L4" s="1"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="18">
         <v>1</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="10"/>
+      <c r="L5" s="1"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="27">
+      <c r="B6" s="30"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="18">
         <v>2</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="20"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="27">
+      <c r="B7" s="30"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="18">
         <v>3</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="20"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="27">
+      <c r="B8" s="30"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="18">
         <v>4</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="27">
+      <c r="B9" s="30"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="18">
         <v>5</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="20"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="26" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="18">
         <v>6</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18" t="s">
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="18">
         <v>7</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="19">
+        <v>8</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="20"/>
-    </row>
-    <row r="12" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="28">
-        <v>8</v>
-      </c>
-      <c r="E12" s="21" t="s">
+      <c r="F12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="19">
+        <v>9</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="20"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="28">
-        <v>9</v>
-      </c>
-      <c r="E13" s="21" t="s">
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="20">
+        <v>10</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="10"/>
-    </row>
-    <row r="14" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="24"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="20">
+        <v>11</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="24"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="19">
         <v>12</v>
       </c>
-      <c r="D14" s="29">
-        <v>10</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="10"/>
-    </row>
-    <row r="15" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="29">
-        <v>11</v>
-      </c>
-      <c r="E15" s="21" t="s">
+      <c r="E16" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="20"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="28">
-        <v>12</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18" t="s">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="10"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="1"/>
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="30"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="30"/>
+      <c r="E25" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="H2:J3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="C5:C9"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="F2:G3"/>
-    <mergeCell ref="H2:J3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="C5:C9"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>